<commit_message>
Add experiment results for missing data reconstruction using ensemble learning
</commit_message>
<xml_diff>
--- a/Experiment_Resulsts/Banks_Missing_Data_Summary.xlsx
+++ b/Experiment_Resulsts/Banks_Missing_Data_Summary.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10715"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/htetnaing/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/htetnaing/Development/htet_mces_bank_data/Experiment_Resulsts/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6943F5-EAFB-AF49-91CB-389381FC6A67}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="460" yWindow="1100" windowWidth="24960" windowHeight="13920" tabRatio="500"/>
+    <workbookView xWindow="460" yWindow="1080" windowWidth="24960" windowHeight="13920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -74,7 +75,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -154,6 +155,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -421,11 +425,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -537,7 +541,7 @@
     </row>
     <row r="6" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -643,7 +647,7 @@
     </row>
     <row r="11" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Successfully reconstructed missing data for both failed banks and survived banks
</commit_message>
<xml_diff>
--- a/Experiment_Resulsts/Banks_Missing_Data_Summary.xlsx
+++ b/Experiment_Resulsts/Banks_Missing_Data_Summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/htetnaing/Development/htet_mces_bank_data/Experiment_Resulsts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\htet_mces_bank_data\Experiment_Resulsts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6943F5-EAFB-AF49-91CB-389381FC6A67}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{471A3771-3D94-479D-8C55-8E130D2DA77C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="460" yWindow="1080" windowWidth="24960" windowHeight="13920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -92,7 +92,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -123,6 +123,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -136,7 +142,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -146,6 +152,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,17 +436,17 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -471,9 +478,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
-      <c r="B3">
+      <c r="B3" s="7">
         <v>1308</v>
       </c>
       <c r="C3">
@@ -485,7 +492,7 @@
       <c r="E3">
         <v>23269</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="7">
         <v>1362</v>
       </c>
       <c r="G3">
@@ -494,7 +501,7 @@
       <c r="H3">
         <v>18512</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="7">
         <v>18512</v>
       </c>
       <c r="J3">
@@ -504,7 +511,7 @@
         <v>1353</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -539,12 +546,12 @@
         <v>1.99</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="1" t="s">
         <v>1</v>
@@ -577,9 +584,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
-      <c r="B8">
+      <c r="B8" s="7">
         <v>1289</v>
       </c>
       <c r="C8">
@@ -591,7 +598,7 @@
       <c r="E8">
         <v>3907</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="7">
         <v>1308</v>
       </c>
       <c r="G8">
@@ -600,7 +607,7 @@
       <c r="H8">
         <v>3739</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="7">
         <v>3739</v>
       </c>
       <c r="J8">
@@ -610,7 +617,7 @@
         <v>1295</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -645,12 +652,12 @@
         <v>20.440000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="1" t="s">
         <v>1</v>
@@ -683,9 +690,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
-      <c r="B13">
+      <c r="B13" s="7">
         <v>19</v>
       </c>
       <c r="C13">
@@ -697,7 +704,7 @@
       <c r="E13">
         <v>19362</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="7">
         <v>54</v>
       </c>
       <c r="G13">
@@ -706,7 +713,7 @@
       <c r="H13">
         <v>14773</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="7">
         <v>14773</v>
       </c>
       <c r="J13">
@@ -716,7 +723,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -751,7 +758,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C17" s="5"/>
     </row>
   </sheetData>

</xml_diff>